<commit_message>
moving stuff into summary
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-07-03.xlsx
+++ b/EC/Train Runs and Enforcements 2016-07-03.xlsx
@@ -2449,7 +2449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2729,6 +2729,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3157,8 +3158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM197"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3553,6 +3554,10 @@
       <c r="N11" s="101"/>
       <c r="O11" s="101"/>
       <c r="P11" s="101"/>
+      <c r="S11" s="111">
+        <f>AVERAGE(S13:S999)</f>
+        <v>0.97241379310344822</v>
+      </c>
     </row>
     <row r="12" spans="1:91" s="5" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">

</xml_diff>